<commit_message>
add slot bundle and edit profile introductions
</commit_message>
<xml_diff>
--- a/docs/prefetch-slot.xlsx
+++ b/docs/prefetch-slot.xlsx
@@ -2319,7 +2319,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
         <v>130</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>49</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>39</v>
@@ -2425,7 +2425,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
         <v>134</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>49</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>39</v>
@@ -2531,7 +2531,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" hidden="true">
+    <row r="18">
       <c r="A18" t="s" s="2">
         <v>141</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>49</v>
       </c>
       <c r="G18" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H18" t="s" s="2">
         <v>39</v>
@@ -2637,7 +2637,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" hidden="true">
+    <row r="19">
       <c r="A19" t="s" s="2">
         <v>147</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>49</v>
       </c>
       <c r="G19" t="s" s="2">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="H19" t="s" s="2">
         <v>39</v>

</xml_diff>

<commit_message>
fix operations and examples
</commit_message>
<xml_diff>
--- a/docs/prefetch-slot.xlsx
+++ b/docs/prefetch-slot.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="160">
   <si>
     <t>Path</t>
   </si>
@@ -310,21 +310,21 @@
     <t>Slot.extension</t>
   </si>
   <si>
+    <t>extensions
+user content</t>
+  </si>
+  <si>
     <t xml:space="preserve">Extension {[]} {[]}
 </t>
   </si>
   <si>
-    <t>Extension</t>
-  </si>
-  <si>
-    <t>An Extension</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value:url}
-</t>
-  </si>
-  <si>
-    <t>open</t>
+    <t>Additional Content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource. In order to make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
   </si>
   <si>
     <t>DomainResource.extension</t>
@@ -333,17 +333,10 @@
     <t>Slot.modifierExtension</t>
   </si>
   <si>
-    <t>extensions
-user content</t>
-  </si>
-  <si>
     <t>Extensions that cannot be ignored</t>
   </si>
   <si>
     <t>May be used to represent additional information that is not part of the basic definition of the resource, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. In order to make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -445,19 +438,19 @@
     <t>Slot.status</t>
   </si>
   <si>
-    <t>busy | free | busy-unavailable | busy-tentative | entered-in-error</t>
-  </si>
-  <si>
-    <t>busy | free | busy-unavailable | busy-tentative | entered-in-error.</t>
+    <t>busy | free | busy-unavailable | entered-in-error</t>
+  </si>
+  <si>
+    <t>busy | free | busy-unavailable | entered-in-error.</t>
   </si>
   <si>
     <t>required</t>
   </si>
   <si>
-    <t>The free/busy status of the slot.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/slotstatus</t>
+    <t>The free/busy status of the slot. This value set is a subset of the the FHIR core Slot value set excluding the 'busy-tentative' concept.</t>
+  </si>
+  <si>
+    <t>http://fhir.org/guides/argonaut-scheduling/ValueSet/argo-slot-status</t>
   </si>
   <si>
     <t>FREEBUSY;FBTYPE=(freeBusyType):19980314T233000Z/19980315T003000Z If the freeBusyType is BUSY, then this value can be excluded</t>
@@ -701,8 +694,8 @@
     <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="75.1953125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="62.44921875" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="126.36328125" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="69.140625" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="18.84375" customWidth="true" bestFit="true"/>
@@ -1592,7 +1585,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -1611,15 +1604,17 @@
         <v>39</v>
       </c>
       <c r="J9" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K9" t="s" s="2">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L9" t="s" s="2">
-        <v>96</v>
-      </c>
-      <c r="M9" s="2"/>
+        <v>97</v>
+      </c>
+      <c r="M9" t="s" s="2">
+        <v>98</v>
+      </c>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
         <v>39</v>
@@ -1656,14 +1651,16 @@
         <v>39</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>97</v>
-      </c>
-      <c r="AB9" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="AB9" t="s" s="2">
+        <v>39</v>
+      </c>
       <c r="AC9" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>98</v>
+        <v>39</v>
       </c>
       <c r="AE9" t="s" s="2">
         <v>99</v>
@@ -1681,7 +1678,7 @@
         <v>39</v>
       </c>
       <c r="AJ9" t="s" s="2">
-        <v>39</v>
+        <v>92</v>
       </c>
       <c r="AK9" t="s" s="2">
         <v>39</v>
@@ -1696,7 +1693,7 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
@@ -1715,16 +1712,16 @@
         <v>39</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="K10" t="s" s="2">
+        <v>101</v>
+      </c>
+      <c r="L10" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="L10" t="s" s="2">
-        <v>103</v>
-      </c>
       <c r="M10" t="s" s="2">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
@@ -1774,7 +1771,7 @@
         <v>39</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>40</v>
@@ -1800,7 +1797,7 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
@@ -1823,13 +1820,13 @@
         <v>50</v>
       </c>
       <c r="J11" t="s" s="2">
+        <v>105</v>
+      </c>
+      <c r="K11" t="s" s="2">
+        <v>106</v>
+      </c>
+      <c r="L11" t="s" s="2">
         <v>107</v>
-      </c>
-      <c r="K11" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="L11" t="s" s="2">
-        <v>109</v>
       </c>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1880,7 +1877,7 @@
         <v>39</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>40</v>
@@ -1901,12 +1898,12 @@
         <v>39</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
@@ -1929,13 +1926,13 @@
         <v>50</v>
       </c>
       <c r="J12" t="s" s="2">
+        <v>110</v>
+      </c>
+      <c r="K12" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="L12" t="s" s="2">
         <v>112</v>
-      </c>
-      <c r="K12" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="L12" t="s" s="2">
-        <v>114</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
@@ -1962,11 +1959,11 @@
         <v>39</v>
       </c>
       <c r="W12" t="s" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="X12" s="2"/>
       <c r="Y12" t="s" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Z12" t="s" s="2">
         <v>39</v>
@@ -1984,7 +1981,7 @@
         <v>39</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>40</v>
@@ -2005,12 +2002,12 @@
         <v>39</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
@@ -2033,13 +2030,13 @@
         <v>50</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
@@ -2070,7 +2067,7 @@
       </c>
       <c r="X13" s="2"/>
       <c r="Y13" t="s" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="Z13" t="s" s="2">
         <v>39</v>
@@ -2088,7 +2085,7 @@
         <v>39</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>40</v>
@@ -2109,12 +2106,12 @@
         <v>39</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
@@ -2137,13 +2134,13 @@
         <v>50</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -2170,14 +2167,14 @@
         <v>39</v>
       </c>
       <c r="W14" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="X14" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="Y14" t="s" s="2">
         <v>125</v>
       </c>
-      <c r="X14" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="Y14" t="s" s="2">
-        <v>127</v>
-      </c>
       <c r="Z14" t="s" s="2">
         <v>39</v>
       </c>
@@ -2194,7 +2191,7 @@
         <v>39</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>40</v>
@@ -2215,12 +2212,12 @@
         <v>39</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -2243,13 +2240,13 @@
         <v>50</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -2276,11 +2273,11 @@
         <v>39</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="X15" s="2"/>
       <c r="Y15" t="s" s="2">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>39</v>
@@ -2298,7 +2295,7 @@
         <v>39</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>40</v>
@@ -2319,12 +2316,12 @@
         <v>39</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
@@ -2347,13 +2344,13 @@
         <v>50</v>
       </c>
       <c r="J16" t="s" s="2">
+        <v>131</v>
+      </c>
+      <c r="K16" t="s" s="2">
+        <v>132</v>
+      </c>
+      <c r="L16" t="s" s="2">
         <v>133</v>
-      </c>
-      <c r="K16" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="L16" t="s" s="2">
-        <v>135</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -2404,7 +2401,7 @@
         <v>39</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>49</v>
@@ -2430,7 +2427,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2456,10 +2453,10 @@
         <v>68</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
@@ -2486,49 +2483,49 @@
         <v>39</v>
       </c>
       <c r="W17" t="s" s="2">
+        <v>137</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>138</v>
+      </c>
+      <c r="Y17" t="s" s="2">
         <v>139</v>
       </c>
-      <c r="X17" t="s" s="2">
+      <c r="Z17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AA17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AB17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AC17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AD17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AE17" t="s" s="2">
+        <v>134</v>
+      </c>
+      <c r="AF17" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AG17" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="AH17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AI17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AJ17" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>140</v>
-      </c>
-      <c r="Y17" t="s" s="2">
-        <v>141</v>
-      </c>
-      <c r="Z17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AA17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AB17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AC17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AD17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AE17" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="AF17" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AG17" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="AH17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AI17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AJ17" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AK17" t="s" s="2">
-        <v>142</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>39</v>
@@ -2536,7 +2533,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -2559,13 +2556,13 @@
         <v>50</v>
       </c>
       <c r="J18" t="s" s="2">
+        <v>142</v>
+      </c>
+      <c r="K18" t="s" s="2">
+        <v>143</v>
+      </c>
+      <c r="L18" t="s" s="2">
         <v>144</v>
-      </c>
-      <c r="K18" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="L18" t="s" s="2">
-        <v>146</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -2616,7 +2613,7 @@
         <v>39</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>49</v>
@@ -2634,15 +2631,15 @@
         <v>39</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -2665,13 +2662,13 @@
         <v>50</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -2722,7 +2719,7 @@
         <v>39</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>49</v>
@@ -2740,15 +2737,15 @@
         <v>39</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2771,13 +2768,13 @@
         <v>39</v>
       </c>
       <c r="J20" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="K20" t="s" s="2">
+        <v>153</v>
+      </c>
+      <c r="L20" t="s" s="2">
         <v>154</v>
-      </c>
-      <c r="K20" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="L20" t="s" s="2">
-        <v>156</v>
       </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
@@ -2785,7 +2782,7 @@
         <v>39</v>
       </c>
       <c r="P20" t="s" s="2">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="Q20" t="s" s="2">
         <v>39</v>
@@ -2830,7 +2827,7 @@
         <v>39</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>40</v>
@@ -2856,7 +2853,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -2879,13 +2876,13 @@
         <v>39</v>
       </c>
       <c r="J21" t="s" s="2">
+        <v>157</v>
+      </c>
+      <c r="K21" t="s" s="2">
+        <v>158</v>
+      </c>
+      <c r="L21" t="s" s="2">
         <v>159</v>
-      </c>
-      <c r="K21" t="s" s="2">
-        <v>160</v>
-      </c>
-      <c r="L21" t="s" s="2">
-        <v>161</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
@@ -2936,7 +2933,7 @@
         <v>39</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>40</v>

</xml_diff>